<commit_message>
missing person, userannouncement and eventlisting changes are made
</commit_message>
<xml_diff>
--- a/public/assets/District_Masters.xlsx
+++ b/public/assets/District_Masters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Desktop\FINAL YEAR PROJECT\Disaster Sentitnel\Disaster-Sentinel\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B615AFFF-9DEE-441D-921F-B5673BF66448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F793DAC-1282-457C-8E9C-FBDEC04AFFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5CD07C28-9675-4FCD-8E82-1132D451C3DF}"/>
   </bookViews>
@@ -2220,9 +2220,6 @@
     <t>Nagaland</t>
   </si>
   <si>
-    <t>mizoram</t>
-  </si>
-  <si>
     <t>Meghalaya</t>
   </si>
   <si>
@@ -2266,6 +2263,9 @@
   </si>
   <si>
     <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
   </si>
 </sst>
 </file>
@@ -2683,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC732886-A14D-45B1-A06A-5B0A65765CF9}">
   <dimension ref="A1:E720"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="C427" sqref="C427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>109</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>110</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>111</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>112</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>113</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>114</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>115</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>116</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="117" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>117</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>118</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>119</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>120</v>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>121</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>122</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>123</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>124</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>125</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>126</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>127</v>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>128</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>129</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>130</v>
@@ -3737,7 +3737,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>131</v>
@@ -3745,7 +3745,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>132</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>133</v>
@@ -3761,7 +3761,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>134</v>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>135</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>136</v>
@@ -3785,7 +3785,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>137</v>
@@ -3793,7 +3793,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>138</v>
@@ -3801,7 +3801,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>139</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>140</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>141</v>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>142</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>143</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>144</v>
@@ -3849,7 +3849,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>145</v>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>146</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>147</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>148</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>149</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>150</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>151</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>152</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>153</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>154</v>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>155</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>156</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>157</v>
@@ -3953,7 +3953,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>158</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>159</v>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>160</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>161</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>162</v>
@@ -3993,7 +3993,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>163</v>
@@ -4001,7 +4001,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>164</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>165</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>166</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>167</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>168</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>169</v>
@@ -4049,7 +4049,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>170</v>
@@ -4057,7 +4057,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>171</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>172</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>173</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>174</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>175</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>176</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>177</v>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>178</v>
@@ -4121,7 +4121,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>179</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>180</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>181</v>
@@ -4145,7 +4145,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>182</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>183</v>
@@ -4161,7 +4161,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>184</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>185</v>
@@ -4177,7 +4177,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>186</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>187</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>188</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>189</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>190</v>
@@ -4217,7 +4217,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>191</v>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>192</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>193</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>194</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>195</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>196</v>
@@ -4265,7 +4265,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>116</v>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>197</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>198</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>199</v>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>200</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>201</v>
@@ -4313,7 +4313,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>202</v>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>203</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>204</v>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>205</v>
@@ -4345,7 +4345,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>206</v>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>207</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>208</v>
@@ -4369,7 +4369,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>209</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>210</v>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>211</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>212</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>213</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>214</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>215</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>216</v>
@@ -4433,7 +4433,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>217</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>218</v>
@@ -4449,7 +4449,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>219</v>
@@ -4457,7 +4457,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>220</v>
@@ -4465,7 +4465,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>221</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>222</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>223</v>
@@ -4489,7 +4489,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>224</v>
@@ -4497,7 +4497,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>225</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>226</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>227</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>228</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>229</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>230</v>
@@ -4545,7 +4545,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>231</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>232</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>233</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>234</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>235</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>236</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>237</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>238</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>239</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>240</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>241</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>242</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>243</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>244</v>
@@ -4657,7 +4657,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>245</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>246</v>
@@ -4673,7 +4673,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>247</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>248</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>249</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>250</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>251</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>252</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>253</v>
@@ -4729,7 +4729,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>254</v>
@@ -4737,7 +4737,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>255</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>256</v>
@@ -4753,7 +4753,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>257</v>
@@ -4761,7 +4761,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>258</v>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>259</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>115</v>
@@ -4785,7 +4785,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>260</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>261</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>262</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>263</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>264</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>265</v>
@@ -4833,7 +4833,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>266</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>267</v>
@@ -4849,7 +4849,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>268</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>269</v>
@@ -4865,7 +4865,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>270</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>271</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>272</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>273</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>274</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>275</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>276</v>
@@ -4921,7 +4921,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>277</v>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>278</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>279</v>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>280</v>
@@ -4953,7 +4953,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>281</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>282</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>283</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>284</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>285</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>286</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>287</v>
@@ -5009,7 +5009,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>288</v>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>289</v>
@@ -5025,7 +5025,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>290</v>
@@ -5033,7 +5033,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>291</v>
@@ -5041,7 +5041,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>292</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>293</v>
@@ -5057,7 +5057,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>294</v>
@@ -5065,7 +5065,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>295</v>
@@ -5073,7 +5073,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>296</v>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>298</v>
@@ -5097,7 +5097,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>299</v>
@@ -5105,7 +5105,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>300</v>
@@ -5113,7 +5113,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>301</v>
@@ -5121,7 +5121,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>302</v>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>303</v>
@@ -5137,7 +5137,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>304</v>
@@ -5145,7 +5145,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>305</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>306</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>307</v>
@@ -5169,7 +5169,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>308</v>
@@ -5177,7 +5177,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>309</v>
@@ -5185,7 +5185,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>310</v>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>311</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>312</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>313</v>
@@ -5217,7 +5217,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>314</v>
@@ -5225,7 +5225,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>315</v>
@@ -5233,7 +5233,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>316</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>317</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>318</v>
@@ -5257,7 +5257,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>319</v>
@@ -5265,7 +5265,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>320</v>
@@ -5273,7 +5273,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>321</v>
@@ -5281,7 +5281,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>322</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>323</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>324</v>
@@ -5305,7 +5305,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>325</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>326</v>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>327</v>
@@ -5329,7 +5329,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>328</v>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>329</v>
@@ -5345,7 +5345,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>330</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>331</v>
@@ -5361,7 +5361,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>332</v>
@@ -5369,7 +5369,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>333</v>
@@ -5377,7 +5377,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>334</v>
@@ -5385,7 +5385,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>335</v>
@@ -5393,7 +5393,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>336</v>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>337</v>
@@ -5409,7 +5409,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>338</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>339</v>
@@ -5425,7 +5425,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>340</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>341</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>342</v>
@@ -5449,7 +5449,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>343</v>
@@ -5457,7 +5457,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>344</v>
@@ -5465,7 +5465,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>345</v>
@@ -5473,7 +5473,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>346</v>
@@ -5481,7 +5481,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>347</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>348</v>
@@ -5497,7 +5497,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>349</v>
@@ -5505,7 +5505,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>350</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>351</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>73</v>
@@ -5529,7 +5529,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>352</v>
@@ -5537,7 +5537,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>353</v>
@@ -5545,7 +5545,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>354</v>
@@ -5553,7 +5553,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B358" s="2" t="s">
         <v>355</v>
@@ -5561,7 +5561,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B359" s="2" t="s">
         <v>356</v>
@@ -5569,7 +5569,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B360" s="2" t="s">
         <v>357</v>
@@ -5577,7 +5577,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B361" s="2" t="s">
         <v>358</v>
@@ -5585,7 +5585,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B362" s="2" t="s">
         <v>359</v>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>360</v>
@@ -5601,7 +5601,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B364" s="2" t="s">
         <v>361</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B365" s="2" t="s">
         <v>362</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>363</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B367" s="2" t="s">
         <v>364</v>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B368" s="2" t="s">
         <v>365</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B369" s="2" t="s">
         <v>366</v>
@@ -5649,7 +5649,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B370" s="2" t="s">
         <v>367</v>
@@ -5657,7 +5657,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B371" s="2" t="s">
         <v>368</v>
@@ -5665,7 +5665,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B372" s="2" t="s">
         <v>369</v>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B373" s="2" t="s">
         <v>370</v>
@@ -5681,7 +5681,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B374" s="2" t="s">
         <v>371</v>
@@ -5689,7 +5689,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B375" s="2" t="s">
         <v>372</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B376" s="2" t="s">
         <v>373</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>130</v>
@@ -5713,7 +5713,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>374</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>375</v>
@@ -5729,7 +5729,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>376</v>
@@ -5737,7 +5737,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>377</v>
@@ -5745,7 +5745,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>378</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>379</v>
@@ -5761,7 +5761,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>380</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>381</v>
@@ -5777,7 +5777,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>382</v>
@@ -5785,7 +5785,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>383</v>
@@ -5793,7 +5793,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>384</v>
@@ -5801,7 +5801,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>385</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B390" s="2" t="s">
         <v>386</v>
@@ -5817,7 +5817,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B391" s="2" t="s">
         <v>387</v>
@@ -5825,7 +5825,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B392" s="2" t="s">
         <v>388</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B393" s="2" t="s">
         <v>389</v>
@@ -5841,7 +5841,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B394" s="2" t="s">
         <v>390</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B395" s="2" t="s">
         <v>391</v>
@@ -5857,7 +5857,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B396" s="2" t="s">
         <v>392</v>
@@ -5865,7 +5865,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A397" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B397" s="2" t="s">
         <v>393</v>
@@ -5873,7 +5873,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A398" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B398" s="2" t="s">
         <v>394</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A399" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B399" s="2" t="s">
         <v>395</v>
@@ -5889,7 +5889,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A400" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B400" s="2" t="s">
         <v>396</v>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A401" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B401" s="2" t="s">
         <v>397</v>
@@ -5905,7 +5905,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B402" s="2" t="s">
         <v>398</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A403" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B403" s="2" t="s">
         <v>399</v>
@@ -5921,7 +5921,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A404" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B404" s="2" t="s">
         <v>400</v>
@@ -5929,7 +5929,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A405" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B405" s="2" t="s">
         <v>401</v>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A406" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B406" s="2" t="s">
         <v>402</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A407" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B407" s="2" t="s">
         <v>403</v>
@@ -5953,7 +5953,7 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A408" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B408" s="2" t="s">
         <v>404</v>
@@ -5961,7 +5961,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B409" s="2" t="s">
         <v>405</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A410" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B410" s="2" t="s">
         <v>406</v>
@@ -5977,7 +5977,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A411" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B411" s="2" t="s">
         <v>407</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A412" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B412" s="2" t="s">
         <v>408</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A413" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B413" s="2" t="s">
         <v>409</v>
@@ -6001,7 +6001,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A414" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B414" s="2" t="s">
         <v>410</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A415" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B415" s="2" t="s">
         <v>411</v>
@@ -6017,7 +6017,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A416" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B416" s="2" t="s">
         <v>412</v>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A417" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B417" s="2" t="s">
         <v>413</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A418" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B418" s="2" t="s">
         <v>414</v>
@@ -6041,7 +6041,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A419" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B419" s="2" t="s">
         <v>415</v>
@@ -6049,7 +6049,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A420" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B420" s="2" t="s">
         <v>416</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B421" s="2" t="s">
         <v>417</v>
@@ -6065,7 +6065,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A422" s="2" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B422" s="2" t="s">
         <v>418</v>

</xml_diff>